<commit_message>
added random transfer of students
</commit_message>
<xml_diff>
--- a/Courses table.xlsx
+++ b/Courses table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malov\PycharmProjects\HueviyAlgosForProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malov\PycharmProjects\elect-gen-core\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -395,7 +395,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +424,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -435,7 +435,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -468,7 +468,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1">
-        <v>30</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -512,7 +512,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added ability to work with both 1st year and 2nd year students
</commit_message>
<xml_diff>
--- a/Courses table.xlsx
+++ b/Courses table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -66,6 +66,18 @@
   </si>
   <si>
     <t>Lambda-Calculus, Algebra, Machinery and Logic for Formal Program Semantics</t>
+  </si>
+  <si>
+    <t>Cross-platform Mobile Development with Flutter</t>
+  </si>
+  <si>
+    <t>Advanced Programming in C/C++ (Russian only)</t>
+  </si>
+  <si>
+    <t>Introduction to Mechanical Engineering</t>
+  </si>
+  <si>
+    <t>Introduction to Electronic and Logic Circuits</t>
   </si>
 </sst>
 </file>
@@ -88,12 +100,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor rgb="FFF4CCCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,10 +126,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -392,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +465,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -457,7 +476,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -479,7 +498,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -490,7 +509,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -501,7 +520,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -523,7 +542,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -534,7 +553,51 @@
         <v>13</v>
       </c>
       <c r="C12" s="1">
-        <v>30</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimizations and bug fixes Deprecated GA Updated CLI Improved efficiency of main algorithm
</commit_message>
<xml_diff>
--- a/Courses table.xlsx
+++ b/Courses table.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efimo\PycharmProjects\elect-gen-core\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malov\PycharmProjects\elect-gen-core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D82022A-CEF6-4018-8235-40EAF9585A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6345" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -67,12 +66,24 @@
   </si>
   <si>
     <t>Lambda-Calculus, Algebra, Machinery and Logic for Formal Program Semantics</t>
+  </si>
+  <si>
+    <t>Cross-platform Mobile Development with Flutter</t>
+  </si>
+  <si>
+    <t>Advanced Programming in C/C++ (Russian only)</t>
+  </si>
+  <si>
+    <t>Introduction to Mechanical Engineering</t>
+  </si>
+  <si>
+    <t>Introduction to Electronic and Logic Circuits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,12 +100,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor rgb="FFF4CCCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -109,10 +126,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -392,11 +410,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +465,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -458,7 +476,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -480,7 +498,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -491,7 +509,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -502,7 +520,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -524,7 +542,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -535,7 +553,51 @@
         <v>13</v>
       </c>
       <c r="C12" s="1">
-        <v>35</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>